<commit_message>
changes to It 3 survey
</commit_message>
<xml_diff>
--- a/Iteration 3/Survey/Survey.xlsx
+++ b/Iteration 3/Survey/Survey.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>Personal Information</t>
   </si>
@@ -108,37 +108,61 @@
     <t>If yes,</t>
   </si>
   <si>
-    <t>Which referencing technique is quicker:</t>
-  </si>
-  <si>
-    <t>Which referencing technique is more confusing:</t>
-  </si>
-  <si>
-    <t>Which referencing technique do you prefer:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Do you think this website is sufficient in illustrating the differences between the two techniques?</t>
-  </si>
-  <si>
     <t xml:space="preserve">No </t>
   </si>
   <si>
-    <t>Is this website close enough in resemblance to a normal news website?</t>
-  </si>
-  <si>
-    <t>Would you prefer not having to use your hands at all, i.e. no button clicking?</t>
-  </si>
-  <si>
-    <t>Would you prefer a different numbering style, e.g. Section 1 numbering, Section 2 numbering?</t>
-  </si>
-  <si>
-    <t>Do you think annotating and referring to sections by colours would be beneficial?</t>
-  </si>
-  <si>
-    <t>What type of internet connectivity do you have?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Would you prefer a program that only runs on your machine and that does not use the internet?</t>
+    <t>Numerical referencing vs. Spoken link names</t>
+  </si>
+  <si>
+    <t>1. Which referencing technique is quicker:</t>
+  </si>
+  <si>
+    <t>2. Which referencing technique is more confusing:</t>
+  </si>
+  <si>
+    <t>3. Which referencing technique do you prefer:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Visual aspects </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4. Do you think this website is sufficient in illustrating the differences between the two techniques of voice referencing?</t>
+  </si>
+  <si>
+    <t>5. Would you prefer a different numbering style, e.g. Section 1 numbering, Section 2 numbering?</t>
+  </si>
+  <si>
+    <t>6. Do you think annotating and referring to sections by colours would be beneficial?</t>
+  </si>
+  <si>
+    <t>7. Is this website close enough in resemblance to a news website?</t>
+  </si>
+  <si>
+    <t>8. Would you like to be able to customize the colour of link highlighting?</t>
+  </si>
+  <si>
+    <t>9. Would being able to zoom in and out of different sections of a webpage with your voice be important to you?</t>
+  </si>
+  <si>
+    <t>User interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10. Do you think it’s reasonable to expect that most elderly would be able to press and hold a button to activate voice recognition? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. Do you like having voice feedback or would you prefer having some other visual form of feedback? </t>
+  </si>
+  <si>
+    <t>Commands</t>
+  </si>
+  <si>
+    <t>13. What type of internet connectivity do you have?</t>
+  </si>
+  <si>
+    <t>14. Would you prefer a complete application that only runs on your machine and does not use the internet (Internet cap consideration)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12. Considering the voice commands (home, backwards, forwards,up,down). Do you think that it is not necessary to have to wait for a confirmation of “yes” or “no” in order to go home, backwards or forwards (or do you think that it would be better if it immediately follows the command it thinks you’ve said?)? </t>
   </si>
 </sst>
 </file>
@@ -170,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,8 +207,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -227,20 +257,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -254,13 +275,29 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J67"/>
+  <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -851,7 +888,7 @@
       </c>
     </row>
     <row r="39" spans="1:10" ht="18.75">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="13" t="s">
         <v>24</v>
       </c>
       <c r="B39" s="8"/>
@@ -859,69 +896,112 @@
       <c r="D39" s="9"/>
       <c r="E39" s="9"/>
       <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
+      <c r="G39" s="14"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9"/>
       <c r="J39" s="9"/>
     </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
-      <c r="F40" s="7"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="12"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
-    </row>
-    <row r="41" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C41" s="3"/>
-      <c r="D41" s="1" t="s">
+    <row r="40" spans="1:10" s="16" customFormat="1" ht="18.75">
+      <c r="A40" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23"/>
+    </row>
+    <row r="41" spans="1:10">
+      <c r="A41" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+    </row>
+    <row r="42" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C42" s="3"/>
+      <c r="D42" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="1" t="s">
+      <c r="E42" s="3"/>
+      <c r="F42" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
-      <c r="A43" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C44" s="3"/>
-      <c r="D44" s="1" t="s">
+    <row r="44" spans="1:10">
+      <c r="A44" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C45" s="3"/>
+      <c r="D45" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="1" t="s">
+      <c r="E45" s="3"/>
+      <c r="F45" s="1" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="47" spans="1:10">
-      <c r="A47" s="10" t="s">
-        <v>32</v>
+      <c r="C47" s="3"/>
+      <c r="D47" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="48" spans="1:10">
-      <c r="C48" s="3"/>
-      <c r="D48" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10">
-      <c r="A50" s="10" t="s">
-        <v>33</v>
-      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:10" ht="18.75">
+      <c r="A49" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="15"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+    </row>
+    <row r="50" spans="1:10" ht="30.75" customHeight="1">
+      <c r="A50" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
     </row>
     <row r="51" spans="1:10" ht="18.75" customHeight="1">
       <c r="C51" s="3"/>
@@ -930,7 +1010,7 @@
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -939,7 +1019,7 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="10" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="18.75" customHeight="1">
@@ -949,7 +1029,7 @@
       </c>
       <c r="E54" s="3"/>
       <c r="F54" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -958,7 +1038,7 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="10" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="18.75" customHeight="1">
@@ -968,7 +1048,7 @@
       </c>
       <c r="E57" s="3"/>
       <c r="F57" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -976,8 +1056,8 @@
       <c r="J57" s="2"/>
     </row>
     <row r="59" spans="1:10">
-      <c r="A59" s="10" t="s">
-        <v>37</v>
+      <c r="A59" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="18.75" customHeight="1">
@@ -987,7 +1067,7 @@
       </c>
       <c r="E60" s="3"/>
       <c r="F60" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -995,8 +1075,8 @@
       <c r="J60" s="2"/>
     </row>
     <row r="62" spans="1:10">
-      <c r="A62" s="10" t="s">
-        <v>38</v>
+      <c r="A62" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="18.75" customHeight="1">
@@ -1006,43 +1086,227 @@
       </c>
       <c r="E63" s="3"/>
       <c r="F63" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
-    <row r="65" spans="1:10" ht="18.75" customHeight="1">
-      <c r="A65" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C67" s="3"/>
-      <c r="D67" s="1" t="s">
+    <row r="65" spans="1:10" ht="27.75" customHeight="1">
+      <c r="A65" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+      <c r="I65" s="20"/>
+      <c r="J65" s="20"/>
+    </row>
+    <row r="66" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C66" s="3"/>
+      <c r="D66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G66" s="2"/>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2"/>
+      <c r="J66" s="2"/>
+    </row>
+    <row r="67" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C67" s="7"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+    </row>
+    <row r="68" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A68" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" s="15"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+    </row>
+    <row r="69" spans="1:10" ht="30" customHeight="1">
+      <c r="A69" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
+      <c r="H69" s="19"/>
+      <c r="I69" s="19"/>
+      <c r="J69" s="19"/>
+    </row>
+    <row r="70" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C70" s="3"/>
+      <c r="D70" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E70" s="3"/>
+      <c r="F70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G70" s="2"/>
+      <c r="H70" s="2"/>
+      <c r="I70" s="2"/>
+      <c r="J70" s="2"/>
+    </row>
+    <row r="71" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C71" s="7"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+    </row>
+    <row r="72" spans="1:10" ht="30" customHeight="1">
+      <c r="A72" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B72" s="19"/>
+      <c r="C72" s="19"/>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
+      <c r="I72" s="19"/>
+      <c r="J72" s="19"/>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="C73" s="3"/>
+      <c r="D73" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="3"/>
+      <c r="F73" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2"/>
+      <c r="I73" s="2"/>
+      <c r="J73" s="2"/>
+    </row>
+    <row r="75" spans="1:10" ht="18.75">
+      <c r="A75" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75" s="15"/>
+      <c r="C75" s="21"/>
+      <c r="D75" s="21"/>
+      <c r="E75" s="21"/>
+      <c r="F75" s="21"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
+      <c r="J75" s="21"/>
+    </row>
+    <row r="76" spans="1:10" ht="60" customHeight="1">
+      <c r="A76" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" s="20"/>
+      <c r="C76" s="20"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="20"/>
+      <c r="I76" s="20"/>
+      <c r="J76" s="20"/>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="C77" s="3"/>
+      <c r="D77" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E77" s="3"/>
+      <c r="F77" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="2"/>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="22"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+    </row>
+    <row r="82" spans="1:10" ht="30" customHeight="1">
+      <c r="A82" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B82" s="19"/>
+      <c r="C82" s="19"/>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="G82" s="19"/>
+      <c r="H82" s="19"/>
+      <c r="I82" s="19"/>
+      <c r="J82" s="19"/>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="C83" s="3"/>
+      <c r="D83" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E83" s="3"/>
+      <c r="F83" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I40:J40"/>
+  <mergeCells count="7">
+    <mergeCell ref="A76:J76"/>
+    <mergeCell ref="A82:J82"/>
+    <mergeCell ref="I41:J41"/>
+    <mergeCell ref="A50:J50"/>
+    <mergeCell ref="A65:J65"/>
+    <mergeCell ref="A69:J69"/>
+    <mergeCell ref="A72:J72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
just moved further down the page
</commit_message>
<xml_diff>
--- a/Iteration 3/Survey/Survey.xlsx
+++ b/Iteration 3/Survey/Survey.xlsx
@@ -278,26 +278,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -592,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J83"/>
+  <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -887,426 +887,426 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="18.75">
-      <c r="A39" s="13" t="s">
+    <row r="47" spans="1:10" ht="18.75">
+      <c r="A47" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B39" s="8"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-      <c r="E39" s="9"/>
-      <c r="F39" s="9"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
-      <c r="J39" s="9"/>
-    </row>
-    <row r="40" spans="1:10" s="16" customFormat="1" ht="18.75">
-      <c r="A40" s="17" t="s">
+      <c r="B47" s="8"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+    </row>
+    <row r="48" spans="1:10" s="15" customFormat="1" ht="18.75">
+      <c r="A48" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="23"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="23"/>
-      <c r="G40" s="23"/>
-      <c r="H40" s="23"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="23"/>
-    </row>
-    <row r="41" spans="1:10">
-      <c r="A41" s="10" t="s">
+      <c r="B48" s="16"/>
+      <c r="C48" s="19"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="19"/>
+      <c r="F48" s="19"/>
+      <c r="G48" s="19"/>
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+      <c r="J48" s="19"/>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="7"/>
-      <c r="E41" s="7"/>
-      <c r="F41" s="7"/>
-      <c r="G41" s="7"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
-    </row>
-    <row r="42" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C42" s="3"/>
-      <c r="D42" s="1" t="s">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+    </row>
+    <row r="50" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C50" s="3"/>
+      <c r="D50" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="1" t="s">
+      <c r="E50" s="3"/>
+      <c r="F50" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
-      <c r="A44" s="10" t="s">
+    <row r="52" spans="1:10">
+      <c r="A52" s="10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C45" s="3"/>
-      <c r="D45" s="1" t="s">
+    <row r="53" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C53" s="3"/>
+      <c r="D53" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="3"/>
-      <c r="F45" s="1" t="s">
+      <c r="E53" s="3"/>
+      <c r="F53" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
-      <c r="A46" s="10" t="s">
+    <row r="54" spans="1:10">
+      <c r="A54" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
-      <c r="C47" s="3"/>
-      <c r="D47" s="1" t="s">
+    <row r="55" spans="1:10">
+      <c r="C55" s="3"/>
+      <c r="D55" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="1" t="s">
+      <c r="E55" s="3"/>
+      <c r="F55" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
-      <c r="C48" s="7"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:10" ht="18.75">
-      <c r="A49" s="15" t="s">
+    <row r="56" spans="1:10">
+      <c r="C56" s="7"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:10" ht="18.75">
+      <c r="A57" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="21"/>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
-    </row>
-    <row r="50" spans="1:10" ht="30.75" customHeight="1">
-      <c r="A50" s="18" t="s">
+      <c r="B57" s="14"/>
+      <c r="C57" s="17"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+    </row>
+    <row r="58" spans="1:10" ht="30.75" customHeight="1">
+      <c r="A58" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-    </row>
-    <row r="51" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C51" s="3"/>
-      <c r="D51" s="1" t="s">
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+    </row>
+    <row r="59" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C59" s="3"/>
+      <c r="D59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="1" t="s">
+      <c r="E59" s="3"/>
+      <c r="F59" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-    </row>
-    <row r="53" spans="1:10">
-      <c r="A53" s="10" t="s">
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+      <c r="J59" s="2"/>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C54" s="3"/>
-      <c r="D54" s="1" t="s">
+    <row r="62" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C62" s="3"/>
+      <c r="D62" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="1" t="s">
+      <c r="E62" s="3"/>
+      <c r="F62" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-    </row>
-    <row r="56" spans="1:10">
-      <c r="A56" s="10" t="s">
+      <c r="G62" s="2"/>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C57" s="3"/>
-      <c r="D57" s="1" t="s">
+    <row r="65" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C65" s="3"/>
+      <c r="D65" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="1" t="s">
+      <c r="E65" s="3"/>
+      <c r="F65" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-    </row>
-    <row r="59" spans="1:10">
-      <c r="A59" s="1" t="s">
+      <c r="G65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
+      <c r="J65" s="2"/>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C60" s="3"/>
-      <c r="D60" s="1" t="s">
+    <row r="68" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C68" s="3"/>
+      <c r="D68" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="1" t="s">
+      <c r="E68" s="3"/>
+      <c r="F68" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" s="1" t="s">
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="18.75" customHeight="1">
-      <c r="C63" s="3"/>
-      <c r="D63" s="1" t="s">
+    <row r="71" spans="1:10" ht="18.75" customHeight="1">
+      <c r="C71" s="3"/>
+      <c r="D71" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="1" t="s">
+      <c r="E71" s="3"/>
+      <c r="F71" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-    </row>
-    <row r="65" spans="1:10" ht="27.75" customHeight="1">
-      <c r="A65" s="20" t="s">
+      <c r="G71" s="2"/>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2"/>
+    </row>
+    <row r="73" spans="1:10" ht="27.75" customHeight="1">
+      <c r="A73" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B65" s="20"/>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20"/>
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="20"/>
-      <c r="H65" s="20"/>
-      <c r="I65" s="20"/>
-      <c r="J65" s="20"/>
-    </row>
-    <row r="66" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C66" s="3"/>
-      <c r="D66" s="1" t="s">
+      <c r="B73" s="20"/>
+      <c r="C73" s="20"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="20"/>
+      <c r="I73" s="20"/>
+      <c r="J73" s="20"/>
+    </row>
+    <row r="74" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C74" s="3"/>
+      <c r="D74" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="1" t="s">
+      <c r="E74" s="3"/>
+      <c r="F74" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-    </row>
-    <row r="67" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C67" s="7"/>
-      <c r="D67" s="1"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="7"/>
-      <c r="H67" s="7"/>
-      <c r="I67" s="7"/>
-      <c r="J67" s="7"/>
-    </row>
-    <row r="68" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A68" s="15" t="s">
+      <c r="G74" s="2"/>
+      <c r="H74" s="2"/>
+      <c r="I74" s="2"/>
+      <c r="J74" s="2"/>
+    </row>
+    <row r="75" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C75" s="7"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+      <c r="I75" s="7"/>
+      <c r="J75" s="7"/>
+    </row>
+    <row r="76" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A76" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="21"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="21"/>
-      <c r="F68" s="21"/>
-      <c r="G68" s="21"/>
-      <c r="H68" s="21"/>
-      <c r="I68" s="21"/>
-      <c r="J68" s="21"/>
-    </row>
-    <row r="69" spans="1:10" ht="30" customHeight="1">
-      <c r="A69" s="20" t="s">
+      <c r="B76" s="14"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+      <c r="F76" s="17"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+      <c r="J76" s="17"/>
+    </row>
+    <row r="77" spans="1:10" ht="30" customHeight="1">
+      <c r="A77" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="19"/>
-      <c r="G69" s="19"/>
-      <c r="H69" s="19"/>
-      <c r="I69" s="19"/>
-      <c r="J69" s="19"/>
-    </row>
-    <row r="70" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C70" s="3"/>
-      <c r="D70" s="1" t="s">
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
+      <c r="J77" s="21"/>
+    </row>
+    <row r="78" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C78" s="3"/>
+      <c r="D78" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E70" s="3"/>
-      <c r="F70" s="1" t="s">
+      <c r="E78" s="3"/>
+      <c r="F78" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
-      <c r="J70" s="2"/>
-    </row>
-    <row r="71" spans="1:10" ht="15.75" customHeight="1">
-      <c r="C71" s="7"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="7"/>
-      <c r="H71" s="7"/>
-      <c r="I71" s="7"/>
-      <c r="J71" s="7"/>
-    </row>
-    <row r="72" spans="1:10" ht="30" customHeight="1">
-      <c r="A72" s="20" t="s">
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+    </row>
+    <row r="79" spans="1:10" ht="15.75" customHeight="1">
+      <c r="C79" s="7"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+    </row>
+    <row r="80" spans="1:10" ht="30" customHeight="1">
+      <c r="A80" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="19"/>
-      <c r="G72" s="19"/>
-      <c r="H72" s="19"/>
-      <c r="I72" s="19"/>
-      <c r="J72" s="19"/>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="C73" s="3"/>
-      <c r="D73" s="1" t="s">
+      <c r="B80" s="21"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
+      <c r="I80" s="21"/>
+      <c r="J80" s="21"/>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="C81" s="3"/>
+      <c r="D81" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="1" t="s">
+      <c r="E81" s="3"/>
+      <c r="F81" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
-    </row>
-    <row r="75" spans="1:10" ht="18.75">
-      <c r="A75" s="15" t="s">
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+    </row>
+    <row r="83" spans="1:10" ht="18.75">
+      <c r="A83" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B75" s="15"/>
-      <c r="C75" s="21"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="21"/>
-      <c r="F75" s="21"/>
-      <c r="G75" s="21"/>
-      <c r="H75" s="21"/>
-      <c r="I75" s="21"/>
-      <c r="J75" s="21"/>
-    </row>
-    <row r="76" spans="1:10" ht="60" customHeight="1">
-      <c r="A76" s="20" t="s">
+      <c r="B83" s="14"/>
+      <c r="C83" s="17"/>
+      <c r="D83" s="17"/>
+      <c r="E83" s="17"/>
+      <c r="F83" s="17"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
+      <c r="J83" s="17"/>
+    </row>
+    <row r="84" spans="1:10" ht="60" customHeight="1">
+      <c r="A84" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="B76" s="20"/>
-      <c r="C76" s="20"/>
-      <c r="D76" s="20"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="20"/>
-      <c r="H76" s="20"/>
-      <c r="I76" s="20"/>
-      <c r="J76" s="20"/>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="C77" s="3"/>
-      <c r="D77" s="1" t="s">
+      <c r="B84" s="20"/>
+      <c r="C84" s="20"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+      <c r="I84" s="20"/>
+      <c r="J84" s="20"/>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="C85" s="3"/>
+      <c r="D85" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="1" t="s">
+      <c r="E85" s="3"/>
+      <c r="F85" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-      <c r="I77" s="2"/>
-      <c r="J77" s="2"/>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" s="1" t="s">
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+    </row>
+    <row r="87" spans="1:10">
+      <c r="A87" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="22"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="22"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-      <c r="I80" s="2"/>
-      <c r="J80" s="2"/>
-    </row>
-    <row r="82" spans="1:10" ht="30" customHeight="1">
-      <c r="A82" s="20" t="s">
+    <row r="88" spans="1:10">
+      <c r="A88" s="2"/>
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="18"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+      <c r="I88" s="2"/>
+      <c r="J88" s="2"/>
+    </row>
+    <row r="90" spans="1:10" ht="30" customHeight="1">
+      <c r="A90" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19"/>
-      <c r="F82" s="19"/>
-      <c r="G82" s="19"/>
-      <c r="H82" s="19"/>
-      <c r="I82" s="19"/>
-      <c r="J82" s="19"/>
-    </row>
-    <row r="83" spans="1:10">
-      <c r="C83" s="3"/>
-      <c r="D83" s="1" t="s">
+      <c r="B90" s="21"/>
+      <c r="C90" s="21"/>
+      <c r="D90" s="21"/>
+      <c r="E90" s="21"/>
+      <c r="F90" s="21"/>
+      <c r="G90" s="21"/>
+      <c r="H90" s="21"/>
+      <c r="I90" s="21"/>
+      <c r="J90" s="21"/>
+    </row>
+    <row r="91" spans="1:10">
+      <c r="C91" s="3"/>
+      <c r="D91" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E83" s="3"/>
-      <c r="F83" s="1" t="s">
+      <c r="E91" s="3"/>
+      <c r="F91" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-      <c r="I83" s="2"/>
-      <c r="J83" s="2"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
+      <c r="I91" s="2"/>
+      <c r="J91" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A76:J76"/>
-    <mergeCell ref="A82:J82"/>
-    <mergeCell ref="I41:J41"/>
-    <mergeCell ref="A50:J50"/>
-    <mergeCell ref="A65:J65"/>
-    <mergeCell ref="A69:J69"/>
-    <mergeCell ref="A72:J72"/>
+    <mergeCell ref="A84:J84"/>
+    <mergeCell ref="A90:J90"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="A58:J58"/>
+    <mergeCell ref="A73:J73"/>
+    <mergeCell ref="A77:J77"/>
+    <mergeCell ref="A80:J80"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>